<commit_message>
From remote: major change
</commit_message>
<xml_diff>
--- a/NPG_Code/Results_NPG_NMF.xlsx
+++ b/NPG_Code/Results_NPG_NMF.xlsx
@@ -5896,6 +5896,11 @@
           <t xml:space="preserve">(1000, 20, 500) </t>
         </is>
       </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(2000, 20, 3000) </t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5944,6 +5949,31 @@
         </is>
       </c>
       <c r="M42" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>Residual</t>
+        </is>
+      </c>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>Objective</t>
+        </is>
+      </c>
+      <c r="U42" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
@@ -5990,6 +6020,26 @@
           <t>NPG1</t>
         </is>
       </c>
+      <c r="Q43" t="n">
+        <v>5</v>
+      </c>
+      <c r="R43" t="n">
+        <v>492</v>
+      </c>
+      <c r="S43" t="n">
+        <v>9.397204605912674e-07</v>
+      </c>
+      <c r="T43" t="n">
+        <v>0</v>
+      </c>
+      <c r="U43" t="n">
+        <v>314.5390538917854</v>
+      </c>
+      <c r="V43" t="inlineStr">
+        <is>
+          <t>NPG1</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="B44" t="n">
@@ -6026,6 +6076,23 @@
           <t>NPG2</t>
         </is>
       </c>
+      <c r="R44" t="n">
+        <v>502</v>
+      </c>
+      <c r="S44" t="n">
+        <v>8.882688004243152e-07</v>
+      </c>
+      <c r="T44" t="n">
+        <v>6.309988116837763e-16</v>
+      </c>
+      <c r="U44" t="n">
+        <v>316.0082668727264</v>
+      </c>
+      <c r="V44" t="inlineStr">
+        <is>
+          <t>NPG2</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="B45" t="n">
@@ -6062,6 +6129,23 @@
           <t>AdPG</t>
         </is>
       </c>
+      <c r="R45" t="n">
+        <v>851</v>
+      </c>
+      <c r="S45" t="n">
+        <v>9.845838062015851e-07</v>
+      </c>
+      <c r="T45" t="n">
+        <v>2.608542985787702e-15</v>
+      </c>
+      <c r="U45" t="n">
+        <v>541.6682452848181</v>
+      </c>
+      <c r="V45" t="inlineStr">
+        <is>
+          <t>AdPG</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="B46" t="n">
@@ -6098,6 +6182,23 @@
           <t>AdaPG[1.5, 0.75]</t>
         </is>
       </c>
+      <c r="R46" t="n">
+        <v>807</v>
+      </c>
+      <c r="S46" t="n">
+        <v>9.82205805444606e-07</v>
+      </c>
+      <c r="T46" t="n">
+        <v>2.306140788350291e-15</v>
+      </c>
+      <c r="U46" t="n">
+        <v>531.8004874568433</v>
+      </c>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t>AdaPG[1.5, 0.75]</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="B47" t="n">
@@ -6134,6 +6235,23 @@
           <t>PG-LS[1.1, 0.5]</t>
         </is>
       </c>
+      <c r="R47" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S47" t="n">
+        <v>2.150239999180207e-05</v>
+      </c>
+      <c r="T47" t="n">
+        <v>2.320169238077946e-12</v>
+      </c>
+      <c r="U47" t="n">
+        <v>613.4432615386322</v>
+      </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t>PG-LS[1.1, 0.5]</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="B48" t="n">
@@ -6166,6 +6284,23 @@
         <v>745.2917287014425</v>
       </c>
       <c r="N48" t="inlineStr">
+        <is>
+          <t>PG-LS[1.2, 0.5]</t>
+        </is>
+      </c>
+      <c r="R48" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S48" t="n">
+        <v>5.587621699419392e-06</v>
+      </c>
+      <c r="T48" t="n">
+        <v>7.41063156743276e-14</v>
+      </c>
+      <c r="U48" t="n">
+        <v>523.4592844676226</v>
+      </c>
+      <c r="V48" t="inlineStr">
         <is>
           <t>PG-LS[1.2, 0.5]</t>
         </is>

</xml_diff>